<commit_message>
event fixes, player remake
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luna\PycharmProjects\first-contact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98896470-8D5A-4AC4-92B2-4B1E2BB668CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070D158D-6912-4C06-8F4A-0F424F50EF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{777C135D-F560-4EBB-9586-EFCFD2AE7990}"/>
   </bookViews>
@@ -471,10 +471,10 @@
     <t>bl3, new races</t>
   </si>
   <si>
-    <t>flak 1, heavy laser 1</t>
-  </si>
-  <si>
     <t>repair arm</t>
+  </si>
+  <si>
+    <t>2x basic flak, 2x heavy laser 1</t>
   </si>
 </sst>
 </file>
@@ -694,6 +694,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,22 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1058,33 +1058,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="16" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="23" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="8" t="s">
         <v>142</v>
       </c>
@@ -1094,12 +1094,12 @@
       <c r="G2" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="19"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="18"/>
       <c r="D3" s="6" t="s">
         <v>139</v>
       </c>
@@ -1117,13 +1117,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="19"/>
       <c r="I4" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1139,7 +1139,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="18"/>
       <c r="C6" s="6" t="s">
         <v>100</v>
       </c>
@@ -1160,7 +1160,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="19"/>
       <c r="I7" s="1" t="s">
         <v>145</v>
       </c>
@@ -1169,7 +1169,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="20"/>
       <c r="I8" s="1" t="s">
         <v>66</v>
       </c>
@@ -1178,7 +1178,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1208,7 +1208,7 @@
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6" t="s">
         <v>127</v>
       </c>
@@ -1228,7 +1228,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1244,7 +1244,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1297,7 +1297,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1329,7 +1329,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
@@ -1369,7 +1369,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1399,7 +1399,7 @@
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="6" t="s">
         <v>51</v>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="6" t="s">
         <v>38</v>
       </c>
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1473,7 +1473,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="6" t="s">
         <v>49</v>
       </c>
@@ -1491,7 +1491,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+      <c r="A23" s="19"/>
       <c r="C23" s="6" t="s">
         <v>125</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1533,7 +1533,7 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="6" t="s">
         <v>105</v>
       </c>
@@ -1545,13 +1545,13 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -1583,7 +1583,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="6" t="s">
         <v>46</v>
       </c>
@@ -1591,15 +1591,15 @@
         <v>66</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M28"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
+      <c r="A29" s="19"/>
     </row>
     <row r="30" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -1631,7 +1631,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="19"/>
       <c r="I32" s="1" t="s">
         <v>66</v>
       </c>
@@ -1653,7 +1653,7 @@
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -1663,7 +1663,7 @@
         <v>53</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E33" s="7">
         <v>4</v>
@@ -1686,7 +1686,7 @@
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1703,7 +1703,7 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -1719,7 +1719,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -1751,7 +1751,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="6" t="s">
         <v>40</v>
       </c>
@@ -1771,7 +1771,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="8" t="s">
         <v>41</v>
       </c>
@@ -1789,7 +1789,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -1819,7 +1819,7 @@
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
         <v>57</v>
@@ -1835,7 +1835,7 @@
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
         <v>56</v>
@@ -1853,16 +1853,16 @@
       </c>
     </row>
     <row r="42" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="25"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="17"/>
       <c r="J42" s="14"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1924,6 +1924,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="A42:H42"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
@@ -1936,15 +1945,6 @@
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A41"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
special pirates, generic events
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -576,9 +576,6 @@
     <t>weak to fires</t>
   </si>
   <si>
-    <t>active: decrease ion timer</t>
-  </si>
-  <si>
     <t>SECTORS</t>
   </si>
   <si>
@@ -609,9 +606,6 @@
     <t>lanius stasis nebula</t>
   </si>
   <si>
-    <t>rock fortified sector</t>
-  </si>
-  <si>
     <t>LEPTOD</t>
   </si>
   <si>
@@ -642,24 +636,9 @@
     <t>pavonian iridescent worlds</t>
   </si>
   <si>
-    <t>pavonian disordered sector</t>
-  </si>
-  <si>
-    <t>leptod weapon test sector</t>
-  </si>
-  <si>
-    <t>slug volatile nebula</t>
-  </si>
-  <si>
     <t>slug home nebula</t>
   </si>
   <si>
-    <t>leptod hidden home nebula</t>
-  </si>
-  <si>
-    <t>rock perilous sector</t>
-  </si>
-  <si>
     <t>engi research hub</t>
   </si>
   <si>
@@ -673,6 +652,27 @@
   </si>
   <si>
     <t>50% to start a fire on damage dealt</t>
+  </si>
+  <si>
+    <t>rock safe haven</t>
+  </si>
+  <si>
+    <t>leptod dimmed space</t>
+  </si>
+  <si>
+    <t>leptod secret lair</t>
+  </si>
+  <si>
+    <t>active: decrease ion timer OR 3 training level</t>
+  </si>
+  <si>
+    <t>pavonian folly</t>
+  </si>
+  <si>
+    <t>rock volatile wasteland</t>
+  </si>
+  <si>
+    <t>slug stormy nebula</t>
   </si>
 </sst>
 </file>
@@ -1042,49 +1042,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1410,14 +1410,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="3.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="3.42578125" style="38" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
     <col min="12" max="12" width="64.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -1425,36 +1425,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="56"/>
-      <c r="B1" s="63" t="s">
+      <c r="A1" s="58"/>
+      <c r="B1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="58" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="63"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="60"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="8" t="s">
         <v>78</v>
       </c>
@@ -1465,20 +1465,20 @@
         <v>145</v>
       </c>
       <c r="H2" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="J2" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="J2" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" s="62"/>
+      <c r="K2" s="66"/>
       <c r="L2" s="12"/>
-      <c r="M2" s="61"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="57"/>
       <c r="D3" s="6" t="s">
         <v>76</v>
       </c>
@@ -1492,26 +1492,26 @@
         <v>8</v>
       </c>
       <c r="H3" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="J3" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
+      <c r="A4" s="58"/>
       <c r="K4" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1530,7 +1530,7 @@
       <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="57"/>
       <c r="C6" s="6" t="s">
         <v>60</v>
       </c>
@@ -1547,16 +1547,16 @@
         <v>8</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="58"/>
       <c r="I7" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>48</v>
@@ -1566,7 +1566,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
+      <c r="A8" s="61"/>
       <c r="K8" s="1" t="s">
         <v>48</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="57" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1597,7 +1597,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1610,7 +1610,7 @@
       <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="6" t="s">
         <v>70</v>
       </c>
@@ -1622,7 +1622,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="38"/>
       <c r="H10" s="40" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="I10" s="40"/>
       <c r="J10" s="6"/>
@@ -1635,7 +1635,7 @@
       <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1652,7 +1652,7 @@
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="58" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1674,7 +1674,7 @@
         <v>8</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>100</v>
@@ -1684,7 +1684,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="6" t="s">
         <v>9</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>85</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>48</v>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1737,7 +1737,7 @@
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="4" t="s">
@@ -1749,7 +1749,7 @@
       <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="G16" s="38"/>
       <c r="H16" s="40"/>
       <c r="I16" s="40" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="2" t="s">
@@ -1774,7 +1774,7 @@
       <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1795,7 +1795,7 @@
       <c r="M17" s="11"/>
     </row>
     <row r="18" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="57" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1817,11 +1817,11 @@
         <v>8</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>103</v>
@@ -1832,7 +1832,7 @@
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1858,7 +1858,7 @@
       <c r="N19" s="11"/>
     </row>
     <row r="20" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
@@ -1879,7 +1879,7 @@
       <c r="M20" s="11"/>
     </row>
     <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1903,7 +1903,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>52</v>
@@ -1914,7 +1914,7 @@
       <c r="M21" s="10"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="6" t="s">
         <v>40</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>29</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>54</v>
@@ -1932,7 +1932,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
+      <c r="A23" s="58"/>
       <c r="J23" s="40"/>
       <c r="K23" s="1" t="s">
         <v>53</v>
@@ -1942,7 +1942,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1963,11 +1963,11 @@
       <c r="G24" s="7">
         <v>8</v>
       </c>
-      <c r="H24" s="67" t="s">
+      <c r="H24" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="I24" s="68"/>
-      <c r="J24" s="55"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="57"/>
       <c r="K24" s="4" t="s">
         <v>56</v>
       </c>
@@ -1975,16 +1975,16 @@
       <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="42" t="s">
         <v>144</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="56"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="58"/>
       <c r="K25" s="1" t="s">
         <v>57</v>
       </c>
@@ -1993,16 +1993,16 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
+      <c r="A26" s="58"/>
       <c r="B26" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="H26" s="62"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="57"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="61"/>
     </row>
     <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="57" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2025,10 +2025,10 @@
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>95</v>
@@ -2039,7 +2039,7 @@
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
+      <c r="A28" s="58"/>
       <c r="B28" s="6" t="s">
         <v>38</v>
       </c>
@@ -2052,7 +2052,7 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
+      <c r="A29" s="58"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -2066,11 +2066,11 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="57" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="54" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>28</v>
@@ -2088,7 +2088,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
@@ -2101,7 +2101,7 @@
       <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
+      <c r="A31" s="58"/>
       <c r="B31" s="6" t="s">
         <v>87</v>
       </c>
@@ -2111,7 +2111,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="38"/>
       <c r="H31" s="40" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="I31" s="40"/>
       <c r="J31" s="6"/>
@@ -2124,7 +2124,7 @@
       <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
@@ -2143,7 +2143,7 @@
       <c r="M32" s="23"/>
     </row>
     <row r="33" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="57" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
@@ -2165,11 +2165,11 @@
         <v>8</v>
       </c>
       <c r="H33" s="40" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I33" s="40"/>
       <c r="J33" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K33" s="26" t="s">
         <v>92</v>
@@ -2178,7 +2178,7 @@
       <c r="M33" s="11"/>
     </row>
     <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
+      <c r="A34" s="58"/>
       <c r="B34" s="44"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -2197,7 +2197,7 @@
       <c r="M34" s="11"/>
     </row>
     <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
+      <c r="A35" s="58"/>
       <c r="B35" s="25"/>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
@@ -2216,8 +2216,8 @@
       <c r="M35" s="23"/>
     </row>
     <row r="36" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
-        <v>165</v>
+      <c r="A36" s="57" t="s">
+        <v>163</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>93</v>
@@ -2239,10 +2239,10 @@
       </c>
       <c r="H36" s="40"/>
       <c r="I36" s="40" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="K36" s="26" t="s">
         <v>98</v>
@@ -2251,12 +2251,12 @@
       <c r="M36" s="11"/>
     </row>
     <row r="37" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="42" t="s">
         <v>143</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -2272,7 +2272,7 @@
       <c r="M37" s="11"/>
     </row>
     <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
+      <c r="A38" s="58"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
@@ -2291,7 +2291,7 @@
       <c r="M38" s="12"/>
     </row>
     <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="57" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="42" t="s">
@@ -2313,7 +2313,7 @@
         <v>8</v>
       </c>
       <c r="H39" s="40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I39" s="40"/>
       <c r="J39" s="24"/>
@@ -2326,7 +2326,7 @@
       <c r="M39" s="10"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
+      <c r="A40" s="58"/>
       <c r="B40" s="44" t="s">
         <v>152</v>
       </c>
@@ -2335,7 +2335,7 @@
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
       <c r="H40" s="44" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J40" s="24"/>
       <c r="K40" s="49" t="s">
@@ -2347,7 +2347,7 @@
       <c r="M40" s="11"/>
     </row>
     <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
+      <c r="A41" s="58"/>
       <c r="B41" s="53"/>
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
@@ -2366,23 +2366,23 @@
       <c r="M41" s="35"/>
     </row>
     <row r="42" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="66"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="60"/>
       <c r="L42" s="14"/>
       <c r="M42" s="14"/>
     </row>
     <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="57" t="s">
         <v>147</v>
       </c>
       <c r="B43" s="17" t="s">
@@ -2413,7 +2413,7 @@
       <c r="M43" s="10"/>
     </row>
     <row r="44" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
+      <c r="A44" s="58"/>
       <c r="B44" s="17" t="s">
         <v>121</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="M44" s="11"/>
     </row>
     <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
+      <c r="A45" s="58"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -2453,11 +2453,11 @@
       <c r="M45" s="12"/>
     </row>
     <row r="46" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+      <c r="A46" s="57" t="s">
         <v>106</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>44</v>
@@ -2486,7 +2486,7 @@
       <c r="M46" s="11"/>
     </row>
     <row r="47" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
+      <c r="A47" s="58"/>
       <c r="B47" s="45" t="s">
         <v>91</v>
       </c>
@@ -2509,7 +2509,7 @@
       <c r="M47" s="11"/>
     </row>
     <row r="48" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
+      <c r="A48" s="61"/>
       <c r="B48" s="34" t="s">
         <v>59</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="M48" s="27"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="57" t="s">
         <v>105</v>
       </c>
       <c r="B49" s="17" t="s">
@@ -2560,7 +2560,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="56"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17" t="s">
         <v>114</v>
@@ -2577,7 +2577,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
+      <c r="A51" s="61"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
@@ -2596,7 +2596,7 @@
       <c r="M51" s="12"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="55" t="s">
+      <c r="A52" s="57" t="s">
         <v>107</v>
       </c>
       <c r="B52" s="17" t="s">
@@ -2626,7 +2626,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="42" t="s">
         <v>112</v>
       </c>
@@ -2642,7 +2642,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
+      <c r="A54" s="61"/>
       <c r="B54" s="43" t="s">
         <v>105</v>
       </c>
@@ -2662,21 +2662,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H24:J26"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A46:A48"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A30:A32"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A46:A48"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="A15:A17"/>
@@ -2685,10 +2681,14 @@
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H24:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
slug events, orchid placeholder
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -44,34 +44,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C36" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>cloaking should limit your reactor by 1 with each use?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>weapons that are stronger than normal but limit your reactor by 1 with each shot</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C39" authorId="0" shapeId="0">
       <text>
         <r>
@@ -115,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="185">
   <si>
     <t>ENGI</t>
   </si>
@@ -522,9 +494,6 @@
     <t>small tp, 1 dmg 2 proj gemini spawning missiles</t>
   </si>
   <si>
-    <t>2x 2 proj 45 radius 10 charge spawner1</t>
-  </si>
-  <si>
     <t>boosting weapons</t>
   </si>
   <si>
@@ -543,9 +512,6 @@
     <t>big tp, repair burst, zoltan bypass, mantis x2, zoltan x2, clonebay2</t>
   </si>
   <si>
-    <t>mind control, 4 proj 60 radius 13 charge spawner2</t>
-  </si>
-  <si>
     <t>50% to get stunned on damage taken</t>
   </si>
   <si>
@@ -609,9 +575,6 @@
     <t>LEPTOD</t>
   </si>
   <si>
-    <t>hyper weapons</t>
-  </si>
-  <si>
     <t>lizard last refuge</t>
   </si>
   <si>
@@ -663,9 +626,6 @@
     <t>leptod secret lair</t>
   </si>
   <si>
-    <t>active: decrease ion timer OR 3 training level</t>
-  </si>
-  <si>
     <t>pavonian folly</t>
   </si>
   <si>
@@ -673,6 +633,15 @@
   </si>
   <si>
     <t>slug stormy nebula</t>
+  </si>
+  <si>
+    <t>active: ?</t>
+  </si>
+  <si>
+    <t>mind control, 4 proj 60 radius 15 charge spawner2</t>
+  </si>
+  <si>
+    <t>2x 2 proj 45 radius 12 charge spawner1</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1410,7 @@
       <c r="F1" s="63"/>
       <c r="G1" s="58"/>
       <c r="H1" s="62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I1" s="63"/>
       <c r="J1" s="58"/>
@@ -1462,16 +1431,16 @@
         <v>79</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H2" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="41" t="s">
         <v>154</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>156</v>
       </c>
       <c r="K2" s="66"/>
       <c r="L2" s="12"/>
@@ -1492,13 +1461,13 @@
         <v>8</v>
       </c>
       <c r="H3" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>73</v>
@@ -1547,7 +1516,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>75</v>
@@ -1556,7 +1525,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="58"/>
       <c r="I7" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>48</v>
@@ -1597,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1622,7 +1591,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="38"/>
       <c r="H10" s="40" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I10" s="40"/>
       <c r="J10" s="6"/>
@@ -1674,13 +1643,13 @@
         <v>8</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>100</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1692,13 +1661,13 @@
         <v>85</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>48</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1710,7 +1679,7 @@
         <v>48</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1737,7 +1706,7 @@
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="4" t="s">
@@ -1762,7 +1731,7 @@
       <c r="G16" s="38"/>
       <c r="H16" s="40"/>
       <c r="I16" s="40" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="2" t="s">
@@ -1817,17 +1786,17 @@
         <v>8</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="M18" s="10"/>
     </row>
@@ -1840,7 +1809,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1852,7 +1821,7 @@
         <v>48</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
@@ -1903,7 +1872,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>52</v>
@@ -1922,7 +1891,7 @@
         <v>29</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>54</v>
@@ -1977,7 +1946,7 @@
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="58"/>
       <c r="B25" s="42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>86</v>
@@ -1989,7 +1958,7 @@
         <v>57</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2025,10 +1994,10 @@
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>95</v>
@@ -2088,7 +2057,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
@@ -2111,7 +2080,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="38"/>
       <c r="H31" s="40" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I31" s="40"/>
       <c r="J31" s="6"/>
@@ -2138,7 +2107,7 @@
         <v>48</v>
       </c>
       <c r="L32" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M32" s="23"/>
     </row>
@@ -2150,7 +2119,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>81</v>
@@ -2165,11 +2134,11 @@
         <v>8</v>
       </c>
       <c r="H33" s="40" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I33" s="40"/>
       <c r="J33" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K33" s="26" t="s">
         <v>92</v>
@@ -2217,7 +2186,7 @@
     </row>
     <row r="36" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="57" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>93</v>
@@ -2239,10 +2208,10 @@
       </c>
       <c r="H36" s="40"/>
       <c r="I36" s="40" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K36" s="26" t="s">
         <v>98</v>
@@ -2253,11 +2222,9 @@
     <row r="37" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="58"/>
       <c r="B37" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>164</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C37" s="44"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -2313,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="H39" s="40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I39" s="40"/>
       <c r="J39" s="24"/>
@@ -2321,28 +2288,28 @@
         <v>48</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="M39" s="10"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="58"/>
       <c r="B40" s="44" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
       <c r="H40" s="44" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J40" s="24"/>
       <c r="K40" s="49" t="s">
         <v>48</v>
       </c>
       <c r="L40" s="46" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="M40" s="11"/>
     </row>
@@ -2383,7 +2350,7 @@
     </row>
     <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>120</v>
@@ -2448,7 +2415,7 @@
         <v>48</v>
       </c>
       <c r="L45" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M45" s="12"/>
     </row>
@@ -2457,7 +2424,7 @@
         <v>106</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>44</v>
@@ -2573,7 +2540,7 @@
         <v>48</v>
       </c>
       <c r="L50" s="31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
events, placeholder player ships
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -29,21 +29,6 @@
     <author>Eugene</author>
   </authors>
   <commentList>
-    <comment ref="H33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>with special backgrounds
-and slug pleasure cruises</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C39" authorId="0" shapeId="0">
       <text>
         <r>
@@ -116,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="153">
   <si>
     <t>ENGI</t>
   </si>
@@ -319,9 +304,6 @@
     <t>deal more damage</t>
   </si>
   <si>
-    <t>hidden</t>
-  </si>
-  <si>
     <t>Kestrel A</t>
   </si>
   <si>
@@ -517,72 +499,6 @@
     <t>weak to fires</t>
   </si>
   <si>
-    <t>SECTORS</t>
-  </si>
-  <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>NEBULA</t>
-  </si>
-  <si>
-    <t>civilian sector</t>
-  </si>
-  <si>
-    <t>rebel controlled</t>
-  </si>
-  <si>
-    <t>uncharted nebula</t>
-  </si>
-  <si>
-    <t>pirate hideout</t>
-  </si>
-  <si>
-    <t>rebel stronghold</t>
-  </si>
-  <si>
-    <t>lanius stasis nebula</t>
-  </si>
-  <si>
-    <t>lizard last refuge</t>
-  </si>
-  <si>
-    <t>zoltan turbulent nebula</t>
-  </si>
-  <si>
-    <t>zoltan perquisition zone</t>
-  </si>
-  <si>
-    <t>lizard ruins</t>
-  </si>
-  <si>
-    <t>lanius resurgence point</t>
-  </si>
-  <si>
-    <t>pavonian iridescent worlds</t>
-  </si>
-  <si>
-    <t>slug home nebula</t>
-  </si>
-  <si>
-    <t>engi research hub</t>
-  </si>
-  <si>
-    <t>engi contested worlds</t>
-  </si>
-  <si>
-    <t>mantis brood worlds</t>
-  </si>
-  <si>
-    <t>overgrown orchid sector</t>
-  </si>
-  <si>
-    <t>slug stormy nebula</t>
-  </si>
-  <si>
     <t>mind control, 4 proj 60 radius 15 charge spawner2</t>
   </si>
   <si>
@@ -622,9 +538,6 @@
     <t>hacking, 2x mini beam</t>
   </si>
   <si>
-    <t>pavonian communities</t>
-  </si>
-  <si>
     <t>2x flak2, ???</t>
   </si>
   <si>
@@ -646,25 +559,7 @@
     <t>active: restore health, cause breach</t>
   </si>
   <si>
-    <t>mantis slaver colonies</t>
-  </si>
-  <si>
-    <t>aquarian dimmed space</t>
-  </si>
-  <si>
-    <t>aquarian secret lair</t>
-  </si>
-  <si>
     <t>flak arty, flak1</t>
-  </si>
-  <si>
-    <t>rock holy sanctuary</t>
-  </si>
-  <si>
-    <t>rock-owned wasteland</t>
-  </si>
-  <si>
-    <t>orchid garden worlds</t>
   </si>
 </sst>
 </file>
@@ -717,7 +612,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -823,19 +718,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -855,22 +737,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -929,7 +800,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -953,12 +824,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -989,12 +854,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1046,52 +905,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1408,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,73 +1265,56 @@
     <col min="3" max="3" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="3.42578125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="1" customWidth="1"/>
-    <col min="12" max="12" width="64.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="3.42578125" style="36" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
-      <c r="B1" s="65" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="58"/>
+      <c r="B1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="62"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="55"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="63" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" s="67"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="68"/>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="69"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
+      <c r="G2" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="56"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="57"/>
       <c r="D3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="6">
         <v>4</v>
@@ -1495,54 +1322,42 @@
       <c r="F3" s="6">
         <v>2</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="36">
         <v>8</v>
       </c>
-      <c r="H3" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="H4" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
-      <c r="K4" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="60"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="M5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="57"/>
       <c r="C6" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="6">
         <v>3</v>
@@ -1550,46 +1365,40 @@
       <c r="F6" s="6">
         <v>2</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="36">
         <v>8</v>
       </c>
-      <c r="I6" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
-      <c r="I7" s="40" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="K8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="H6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="60"/>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>8</v>
@@ -1603,21 +1412,16 @@
       <c r="G9" s="7">
         <v>6</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="I9" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
       <c r="B10" s="6" t="s">
         <v>65</v>
       </c>
@@ -1627,39 +1431,31 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="60"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="20" t="s">
+      <c r="G11" s="37"/>
+      <c r="H11" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="21"/>
-      <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="I11" s="21"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="58" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1677,51 +1473,45 @@
       <c r="F12" s="6">
         <v>2</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="36">
         <v>8</v>
       </c>
-      <c r="I12" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="H12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
       <c r="B13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+        <v>79</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
+      <c r="H14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1742,23 +1532,16 @@
       <c r="G15" s="7">
         <v>8</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
+      <c r="I15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1768,41 +1551,35 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L16" s="11" t="s">
+      <c r="G16" s="36"/>
+      <c r="H16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M16" s="11"/>
-    </row>
-    <row r="17" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="58"/>
       <c r="B17" s="6" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="1" t="s">
+      <c r="G17" s="36"/>
+      <c r="H17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="M17" s="11"/>
-    </row>
-    <row r="18" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1823,70 +1600,57 @@
       <c r="G18" s="7">
         <v>8</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+      <c r="H18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="58"/>
       <c r="B19" s="6" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-    </row>
-    <row r="20" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
       <c r="B20" s="6" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="2" t="s">
+      <c r="G20" s="36"/>
+      <c r="H20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="L20" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="M20" s="11"/>
-    </row>
-    <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1907,56 +1671,47 @@
       <c r="G21" s="7">
         <v>8</v>
       </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="K21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="I21" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M21" s="10"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
       <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="K22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L22" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="1" t="s">
+      <c r="I22" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="58"/>
+      <c r="H23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="60" t="s">
+    <row r="24" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>22</v>
@@ -1970,46 +1725,35 @@
       <c r="G24" s="7">
         <v>8</v>
       </c>
-      <c r="H24" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="73"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="43" t="s">
-        <v>158</v>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
+      <c r="B25" s="39" t="s">
+        <v>135</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="63"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L25" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
-      <c r="B26" s="43" t="s">
+      <c r="I25" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="64"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="62"/>
-    </row>
-    <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
+    </row>
+    <row r="27" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2030,62 +1774,52 @@
       <c r="G27" s="7">
         <v>8</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="K27" s="4" t="s">
+      <c r="H27" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="L27" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="M27" s="10"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="58"/>
       <c r="B28" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="O28"/>
-    </row>
-    <row r="29" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="H28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L28"/>
+    </row>
+    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58"/>
       <c r="B29" s="18" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="18"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-    </row>
-    <row r="30" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="60" t="s">
-        <v>174</v>
+      <c r="G29" s="37"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="57" t="s">
+        <v>150</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E30" s="24">
         <v>3</v>
@@ -2093,71 +1827,58 @@
       <c r="F30" s="24">
         <v>2</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="36">
         <v>6</v>
       </c>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="K30" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-    </row>
-    <row r="31" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
-      <c r="B31" s="53" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="43" t="s">
+      <c r="H30" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="58"/>
+      <c r="B31" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="39" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-    </row>
-    <row r="32" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="58"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="M32" s="12"/>
-    </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="60" t="s">
+      <c r="G32" s="37"/>
+      <c r="H32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="54" t="s">
-        <v>173</v>
+      <c r="B33" s="50" t="s">
+        <v>149</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>26</v>
@@ -2171,73 +1892,60 @@
       <c r="G33" s="7">
         <v>8</v>
       </c>
-      <c r="H33" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L33" s="10" t="s">
+      <c r="H33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="M33" s="10"/>
-    </row>
-    <row r="34" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="61"/>
-      <c r="B34" s="43" t="s">
-        <v>159</v>
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="58"/>
+      <c r="B34" s="39" t="s">
+        <v>136</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="I34" s="40"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L34" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="M34" s="11"/>
-    </row>
-    <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="61"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="58"/>
       <c r="B35" s="25"/>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
       <c r="E35" s="25"/>
       <c r="F35" s="25"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L35" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="M35" s="23"/>
-    </row>
-    <row r="36" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="60" t="s">
+      <c r="G35" s="37"/>
+      <c r="H35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="J35" s="23"/>
+    </row>
+    <row r="36" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="57" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>121</v>
+        <v>138</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>120</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="24">
         <v>4</v>
@@ -2245,72 +1953,59 @@
       <c r="F36" s="24">
         <v>2</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="36">
         <v>8</v>
       </c>
-      <c r="H36" s="40" t="s">
-        <v>143</v>
-      </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="K36" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-    </row>
-    <row r="37" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="61"/>
-      <c r="B37" s="43"/>
+      <c r="H36" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="58"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="L37" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="M37" s="11"/>
-    </row>
-    <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="58"/>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="L38" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="M38" s="23"/>
-    </row>
-    <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="60" t="s">
+      <c r="G38" s="37"/>
+      <c r="H38" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="J38" s="23"/>
+    </row>
+    <row r="39" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="42" t="s">
-        <v>118</v>
+      <c r="C39" s="38" t="s">
+        <v>117</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E39" s="24">
         <v>4</v>
@@ -2318,90 +2013,75 @@
       <c r="F39" s="24">
         <v>2</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="36">
         <v>8</v>
       </c>
-      <c r="H39" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="I39" s="59" t="s">
-        <v>153</v>
-      </c>
-      <c r="J39" s="24"/>
-      <c r="K39" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="L39" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="M39" s="10"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="61"/>
-      <c r="B40" s="43" t="s">
-        <v>132</v>
+      <c r="H39" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="J39" s="10"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="58"/>
+      <c r="B40" s="39" t="s">
+        <v>131</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
-      <c r="H40" s="43"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="L40" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="M40" s="11"/>
-    </row>
-    <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="61"/>
-      <c r="B41" s="52"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="41"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="L41" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="71"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-    </row>
-    <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="60" t="s">
-        <v>162</v>
+      <c r="H40" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="I40" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="58"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="I41" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="J41" s="33"/>
+    </row>
+    <row r="42" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="57" t="s">
+        <v>139</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E43" s="7">
         <v>2</v>
@@ -2412,142 +2092,124 @@
       <c r="G43" s="7">
         <v>6</v>
       </c>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-    </row>
-    <row r="44" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="61"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="58"/>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="L44" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="M44" s="11"/>
-    </row>
-    <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="61"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J44" s="11"/>
+    </row>
+    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="58"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L45" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="M45" s="12"/>
-    </row>
-    <row r="46" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="60" t="s">
+      <c r="G45" s="37"/>
+      <c r="H45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J45" s="12"/>
+    </row>
+    <row r="46" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="31">
+        <v>3</v>
+      </c>
+      <c r="F46" s="31">
+        <v>2</v>
+      </c>
+      <c r="G46" s="36">
+        <v>6</v>
+      </c>
+      <c r="H46" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="58"/>
+      <c r="B47" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="60"/>
+      <c r="B48" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J48" s="27"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="B46" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="33">
-        <v>3</v>
-      </c>
-      <c r="F46" s="33">
-        <v>2</v>
-      </c>
-      <c r="G46" s="38">
-        <v>6</v>
-      </c>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="L46" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="M46" s="11"/>
-    </row>
-    <row r="47" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="61"/>
-      <c r="B47" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="L47" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="M47" s="11"/>
-    </row>
-    <row r="48" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="62"/>
-      <c r="B48" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L48" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="M48" s="27"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="60" t="s">
-        <v>101</v>
-      </c>
       <c r="B49" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="38" t="s">
         <v>58</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E49" s="17">
         <v>3</v>
@@ -2555,60 +2217,55 @@
       <c r="F49" s="17">
         <v>3</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="36">
         <v>6</v>
       </c>
-      <c r="J49" s="17"/>
-      <c r="K49" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L49" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="61"/>
-      <c r="B50" s="43"/>
+      <c r="H49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="58"/>
+      <c r="B50" s="39"/>
       <c r="C50" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
-      <c r="J50" s="17"/>
-      <c r="K50" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L50" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="62"/>
-      <c r="B51" s="52"/>
+      <c r="H50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="60"/>
+      <c r="B51" s="48"/>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="18"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="60" t="s">
-        <v>160</v>
+      <c r="G51" s="37"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="57" t="s">
+        <v>137</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="38" t="s">
         <v>57</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E52" s="17">
         <v>3</v>
@@ -2616,134 +2273,104 @@
       <c r="F52" s="17">
         <v>3</v>
       </c>
-      <c r="G52" s="38">
+      <c r="G52" s="36">
         <v>4</v>
       </c>
-      <c r="J52" s="17"/>
-      <c r="K52" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L52" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="61"/>
+      <c r="H52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="58"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L53" s="31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="62"/>
+      <c r="H53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I53" s="29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="60"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L54" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="M54" s="12"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C55" s="42" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="55"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C58" s="42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L59" s="1"/>
-    </row>
-    <row r="60" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="56"/>
-      <c r="B60" s="58"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="58"/>
-      <c r="L60" s="55"/>
-      <c r="M60" s="55"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C61" s="42" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="56"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="58"/>
-      <c r="L63" s="55"/>
-      <c r="M63" s="55"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I54" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="J54" s="12"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="52"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="54"/>
+      <c r="I57" s="51"/>
+      <c r="J57" s="51"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C58" s="38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="52"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="54"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="51"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C61" s="38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="52"/>
+      <c r="B63" s="54"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="54"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="54"/>
+      <c r="G63" s="54"/>
+      <c r="I63" s="51"/>
+      <c r="J63" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H24:J26"/>
+  <mergeCells count="25">
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A52:A54"/>
-    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A3:A5"/>
@@ -2752,6 +2379,20 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A30:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>